<commit_message>
Restore pemasaran with original
</commit_message>
<xml_diff>
--- a/Rule Konversi.xlsx
+++ b/Rule Konversi.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229647A9-3A3A-40A4-892C-FB4B3D76E97C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Rule" sheetId="5" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="160">
   <si>
     <t>Pancasila dan Kewarganegaraan</t>
   </si>
@@ -495,16 +494,13 @@
   </si>
   <si>
     <t>Voice Processing (OPTIONAL SUBJECT 2)</t>
-  </si>
-  <si>
-    <t>BAHASA ARAB MAHARAH KITABAH I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -762,14 +758,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -816,7 +804,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -848,27 +836,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -900,24 +870,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1093,14 +1045,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G188"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:G17"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I177" sqref="I177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -1114,7 +1066,7 @@
     <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="30" customFormat="1">
       <c r="A1" s="28">
         <v>1</v>
       </c>
@@ -1137,7 +1089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="30" customFormat="1">
       <c r="A2" s="28">
         <v>2</v>
       </c>
@@ -1160,7 +1112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="30" customFormat="1">
       <c r="A3" s="28">
         <v>3</v>
       </c>
@@ -1183,7 +1135,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="30" customFormat="1">
       <c r="A4" s="28">
         <v>4</v>
       </c>
@@ -1206,7 +1158,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="33" customFormat="1">
       <c r="A5" s="31">
         <v>5</v>
       </c>
@@ -1229,7 +1181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="33" customFormat="1">
       <c r="A6" s="31">
         <v>6</v>
       </c>
@@ -1252,7 +1204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="30" customFormat="1">
       <c r="A7" s="28">
         <v>7</v>
       </c>
@@ -1275,7 +1227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="33" customFormat="1">
       <c r="A8" s="31">
         <v>8</v>
       </c>
@@ -1298,7 +1250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="33" customFormat="1">
       <c r="A9" s="31">
         <v>9</v>
       </c>
@@ -1321,7 +1273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="30" customFormat="1">
       <c r="A10" s="28">
         <v>10</v>
       </c>
@@ -1344,7 +1296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="33" customFormat="1">
       <c r="A11" s="31">
         <v>11</v>
       </c>
@@ -1367,7 +1319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="33" customFormat="1">
       <c r="A12" s="31">
         <v>12</v>
       </c>
@@ -1390,7 +1342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="30" customFormat="1">
       <c r="A13" s="28">
         <v>13</v>
       </c>
@@ -1413,7 +1365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="30" customFormat="1">
       <c r="A14" s="28">
         <v>14</v>
       </c>
@@ -1436,7 +1388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="30" customFormat="1">
       <c r="A15" s="28">
         <v>15</v>
       </c>
@@ -1459,7 +1411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="30" customFormat="1">
       <c r="A16" s="28">
         <v>16</v>
       </c>
@@ -1482,7 +1434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="30" customFormat="1">
       <c r="A17" s="28">
         <v>17</v>
       </c>
@@ -1496,16 +1448,16 @@
         <v>1</v>
       </c>
       <c r="E17" s="28">
-        <v>1700112</v>
+        <v>1400113</v>
       </c>
       <c r="F17" s="29" t="s">
-        <v>160</v>
+        <v>13</v>
       </c>
       <c r="G17" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" s="30" customFormat="1">
       <c r="A18" s="28">
         <v>18</v>
       </c>
@@ -1528,7 +1480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" s="30" customFormat="1">
       <c r="A19" s="28">
         <v>19</v>
       </c>
@@ -1551,7 +1503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" s="30" customFormat="1">
       <c r="A20" s="28">
         <v>20</v>
       </c>
@@ -1574,7 +1526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="30" customFormat="1">
       <c r="A21" s="28">
         <v>21</v>
       </c>
@@ -1597,7 +1549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" s="33" customFormat="1">
       <c r="A22" s="31">
         <v>22</v>
       </c>
@@ -1620,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" s="18" customFormat="1">
       <c r="A23" s="16">
         <v>23</v>
       </c>
@@ -1643,7 +1595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" s="18" customFormat="1">
       <c r="A24" s="16">
         <v>24</v>
       </c>
@@ -1666,7 +1618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="18" customFormat="1">
       <c r="A25" s="16">
         <v>25</v>
       </c>
@@ -1689,7 +1641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="18" customFormat="1">
       <c r="A26" s="16">
         <v>26</v>
       </c>
@@ -1712,7 +1664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" s="18" customFormat="1">
       <c r="A27" s="16">
         <v>27</v>
       </c>
@@ -1735,7 +1687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" s="18" customFormat="1">
       <c r="A28" s="16">
         <v>28</v>
       </c>
@@ -1758,7 +1710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" s="21" customFormat="1">
       <c r="A29" s="19">
         <v>29</v>
       </c>
@@ -1781,7 +1733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="21" customFormat="1">
       <c r="A30" s="19">
         <v>30</v>
       </c>
@@ -1804,7 +1756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="18" customFormat="1">
       <c r="A31" s="16">
         <v>31</v>
       </c>
@@ -1827,7 +1779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" s="21" customFormat="1">
       <c r="A32" s="19">
         <v>32</v>
       </c>
@@ -1850,7 +1802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" s="21" customFormat="1">
       <c r="A33" s="19">
         <v>33</v>
       </c>
@@ -1873,7 +1825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" s="18" customFormat="1">
       <c r="A34" s="16">
         <v>34</v>
       </c>
@@ -1896,7 +1848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" s="18" customFormat="1">
       <c r="A35" s="16">
         <v>35</v>
       </c>
@@ -1919,7 +1871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" s="18" customFormat="1">
       <c r="A36" s="16">
         <v>36</v>
       </c>
@@ -1942,7 +1894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="18" customFormat="1">
       <c r="A37" s="16">
         <v>37</v>
       </c>
@@ -1965,7 +1917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" s="18" customFormat="1">
       <c r="A38" s="16">
         <v>38</v>
       </c>
@@ -1979,16 +1931,16 @@
         <v>1</v>
       </c>
       <c r="E38" s="16">
-        <v>1700112</v>
+        <v>1400113</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>160</v>
+        <v>13</v>
       </c>
       <c r="G38" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" s="18" customFormat="1">
       <c r="A39" s="16">
         <v>39</v>
       </c>
@@ -2011,7 +1963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" s="18" customFormat="1">
       <c r="A40" s="16">
         <v>40</v>
       </c>
@@ -2034,7 +1986,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" s="18" customFormat="1">
       <c r="A41" s="16">
         <v>41</v>
       </c>
@@ -2057,7 +2009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" s="18" customFormat="1">
       <c r="A42" s="16">
         <v>42</v>
       </c>
@@ -2080,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" s="21" customFormat="1">
       <c r="A43" s="19">
         <v>43</v>
       </c>
@@ -2103,7 +2055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" s="15" customFormat="1">
       <c r="A44" s="13">
         <v>44</v>
       </c>
@@ -2126,7 +2078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" s="15" customFormat="1">
       <c r="A45" s="13">
         <v>45</v>
       </c>
@@ -2149,7 +2101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" s="15" customFormat="1">
       <c r="A46" s="13">
         <v>46</v>
       </c>
@@ -2172,7 +2124,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" s="15" customFormat="1">
       <c r="A47" s="13">
         <v>47</v>
       </c>
@@ -2195,7 +2147,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" s="15" customFormat="1">
       <c r="A48" s="13">
         <v>48</v>
       </c>
@@ -2218,7 +2170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" s="15" customFormat="1">
       <c r="A49" s="13">
         <v>49</v>
       </c>
@@ -2241,7 +2193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" s="15" customFormat="1">
       <c r="A50" s="13">
         <v>50</v>
       </c>
@@ -2264,7 +2216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" s="15" customFormat="1">
       <c r="A51" s="13">
         <v>51</v>
       </c>
@@ -2287,7 +2239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" s="15" customFormat="1">
       <c r="A52" s="13">
         <v>52</v>
       </c>
@@ -2310,7 +2262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" s="15" customFormat="1">
       <c r="A53" s="13">
         <v>53</v>
       </c>
@@ -2333,7 +2285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" s="15" customFormat="1">
       <c r="A54" s="13">
         <v>54</v>
       </c>
@@ -2356,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" s="15" customFormat="1">
       <c r="A55" s="13">
         <v>55</v>
       </c>
@@ -2379,7 +2331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" s="15" customFormat="1">
       <c r="A56" s="13">
         <v>56</v>
       </c>
@@ -2402,7 +2354,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" s="15" customFormat="1">
       <c r="A57" s="13">
         <v>57</v>
       </c>
@@ -2416,16 +2368,16 @@
         <v>1</v>
       </c>
       <c r="E57" s="13">
-        <v>1700112</v>
+        <v>1400113</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>160</v>
+        <v>13</v>
       </c>
       <c r="G57" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" s="15" customFormat="1">
       <c r="A58" s="13">
         <v>58</v>
       </c>
@@ -2448,7 +2400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" s="15" customFormat="1">
       <c r="A59" s="13">
         <v>59</v>
       </c>
@@ -2471,7 +2423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" s="15" customFormat="1">
       <c r="A60" s="13">
         <v>60</v>
       </c>
@@ -2494,7 +2446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" s="15" customFormat="1">
       <c r="A61" s="13">
         <v>61</v>
       </c>
@@ -2517,271 +2469,271 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="13">
+    <row r="62" spans="1:7">
+      <c r="A62" s="1">
         <v>62</v>
       </c>
-      <c r="B62" s="13">
-        <v>1700112</v>
-      </c>
-      <c r="C62" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="D62" s="13">
-        <v>1</v>
-      </c>
-      <c r="E62" s="13">
-        <v>1700112</v>
-      </c>
-      <c r="F62" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="G62" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B62" s="1">
+        <v>765208</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" s="1">
+        <v>2</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1565001</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G62" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="1">
         <v>63</v>
       </c>
       <c r="B63" s="1">
-        <v>765208</v>
+        <v>765201</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D63" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E63" s="1">
-        <v>1565001</v>
+        <v>1565002</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G63" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="1">
         <v>64</v>
       </c>
       <c r="B64" s="1">
-        <v>765201</v>
+        <v>765209</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D64" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E64" s="1">
-        <v>1565002</v>
+        <v>1565003</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="G64" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7">
       <c r="A65" s="1">
         <v>65</v>
       </c>
       <c r="B65" s="1">
-        <v>765209</v>
+        <v>765204</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D65" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E65" s="1">
-        <v>1565003</v>
+        <v>1565004</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="G65" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7">
       <c r="A66" s="1">
         <v>66</v>
       </c>
       <c r="B66" s="1">
-        <v>765204</v>
+        <v>765203</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D66" s="1">
         <v>3</v>
       </c>
       <c r="E66" s="1">
-        <v>1565004</v>
+        <v>1565005</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G66" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="1">
         <v>67</v>
       </c>
       <c r="B67" s="1">
-        <v>765203</v>
+        <v>765210</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D67" s="1">
         <v>3</v>
       </c>
       <c r="E67" s="1">
-        <v>1565005</v>
+        <v>1565006</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G67" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="1">
         <v>68</v>
       </c>
       <c r="B68" s="1">
-        <v>765210</v>
+        <v>765211</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D68" s="1">
         <v>3</v>
       </c>
       <c r="E68" s="1">
-        <v>1565006</v>
+        <v>1565007</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G68" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="1">
         <v>69</v>
       </c>
       <c r="B69" s="1">
-        <v>765211</v>
+        <v>765216</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D69" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E69" s="1">
-        <v>1565007</v>
+        <v>1565008</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="G69" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="1">
         <v>70</v>
       </c>
       <c r="B70" s="1">
-        <v>765216</v>
+        <v>765206</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D70" s="1">
         <v>2</v>
       </c>
       <c r="E70" s="1">
-        <v>1565008</v>
+        <v>1565009</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="G70" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="1">
         <v>71</v>
       </c>
       <c r="B71" s="1">
-        <v>765206</v>
+        <v>765212</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D71" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E71" s="1">
-        <v>1565009</v>
+        <v>1565010</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G71" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" s="1">
         <v>72</v>
       </c>
       <c r="B72" s="1">
-        <v>765212</v>
+        <v>765214</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D72" s="1">
         <v>3</v>
       </c>
-      <c r="E72" s="1">
-        <v>1565010</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G72" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E72" s="5">
+        <v>1565011</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G72" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="1">
         <v>73</v>
       </c>
-      <c r="B73" s="1">
-        <v>765214</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D73" s="1">
-        <v>3</v>
+      <c r="B73" s="7">
+        <v>765311</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D73" s="7">
+        <v>2</v>
       </c>
       <c r="E73" s="5">
         <v>1565011</v>
@@ -2793,38 +2745,38 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" s="11" customFormat="1">
       <c r="A74" s="1">
         <v>74</v>
       </c>
       <c r="B74" s="7">
-        <v>765311</v>
+        <v>765219</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D74" s="7">
-        <v>2</v>
-      </c>
-      <c r="E74" s="5">
-        <v>1565011</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="G74" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="E74" s="9">
+        <v>1565012</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G74" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="11" customFormat="1">
       <c r="A75" s="1">
         <v>75</v>
       </c>
       <c r="B75" s="7">
-        <v>765219</v>
+        <v>765217</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D75" s="7">
         <v>3</v>
@@ -2839,87 +2791,87 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7">
       <c r="A76" s="1">
         <v>76</v>
       </c>
-      <c r="B76" s="7">
-        <v>765217</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D76" s="7">
-        <v>3</v>
-      </c>
-      <c r="E76" s="9">
-        <v>1565012</v>
-      </c>
-      <c r="F76" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G76" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B76" s="1">
+        <v>765205</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D76" s="1">
+        <v>2</v>
+      </c>
+      <c r="E76" s="1">
+        <v>1565013</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G76" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" s="1">
         <v>77</v>
       </c>
       <c r="B77" s="1">
-        <v>765205</v>
+        <v>765306</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D77" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E77" s="1">
-        <v>1565013</v>
+        <v>1565014</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G77" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" s="11" customFormat="1">
       <c r="A78" s="1">
         <v>78</v>
       </c>
-      <c r="B78" s="1">
-        <v>765306</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D78" s="1">
-        <v>3</v>
-      </c>
-      <c r="E78" s="1">
-        <v>1565014</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G78" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B78" s="7">
+        <v>765309</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D78" s="7">
+        <v>2</v>
+      </c>
+      <c r="E78" s="9">
+        <v>1565015</v>
+      </c>
+      <c r="F78" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G78" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" s="11" customFormat="1">
       <c r="A79" s="1">
         <v>79</v>
       </c>
       <c r="B79" s="7">
-        <v>765309</v>
+        <v>765312</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D79" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E79" s="9">
         <v>1565015</v>
@@ -2931,375 +2883,375 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7">
       <c r="A80" s="1">
         <v>80</v>
       </c>
-      <c r="B80" s="7">
-        <v>765312</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D80" s="7">
-        <v>3</v>
-      </c>
-      <c r="E80" s="9">
-        <v>1565015</v>
-      </c>
-      <c r="F80" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G80" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B80" s="1">
+        <v>765302</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D80" s="1">
+        <v>3</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1565016</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G80" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="1">
         <v>81</v>
       </c>
       <c r="B81" s="1">
-        <v>765302</v>
+        <v>765218</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D81" s="1">
         <v>3</v>
       </c>
       <c r="E81" s="1">
-        <v>1565016</v>
+        <v>1565017</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="G81" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="1">
         <v>82</v>
       </c>
       <c r="B82" s="1">
-        <v>765218</v>
+        <v>765301</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D82" s="1">
         <v>3</v>
       </c>
       <c r="E82" s="1">
-        <v>1565017</v>
+        <v>1565018</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="G82" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7">
       <c r="A83" s="1">
         <v>83</v>
       </c>
       <c r="B83" s="1">
-        <v>765301</v>
+        <v>765303</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D83" s="1">
         <v>3</v>
       </c>
       <c r="E83" s="1">
-        <v>1565018</v>
+        <v>1565019</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G83" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7">
       <c r="A84" s="1">
         <v>84</v>
       </c>
       <c r="B84" s="1">
-        <v>765303</v>
+        <v>765313</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D84" s="1">
         <v>3</v>
       </c>
       <c r="E84" s="1">
-        <v>1565019</v>
+        <v>1565020</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="G84" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" s="1">
         <v>85</v>
       </c>
       <c r="B85" s="1">
-        <v>765313</v>
+        <v>765213</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D85" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E85" s="1">
-        <v>1565020</v>
+        <v>1565021</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="G85" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" s="1">
         <v>86</v>
       </c>
       <c r="B86" s="1">
-        <v>765213</v>
+        <v>765305</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D86" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E86" s="1">
-        <v>1565021</v>
+        <v>1565022</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="G86" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7">
       <c r="A87" s="1">
         <v>87</v>
       </c>
       <c r="B87" s="1">
-        <v>765305</v>
+        <v>765307</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D87" s="1">
         <v>3</v>
       </c>
       <c r="E87" s="1">
-        <v>1565022</v>
+        <v>1565023</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="G87" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7">
       <c r="A88" s="1">
         <v>88</v>
       </c>
       <c r="B88" s="1">
-        <v>765307</v>
+        <v>765207</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D88" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E88" s="1">
-        <v>1565023</v>
+        <v>1565024</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>141</v>
+        <v>82</v>
       </c>
       <c r="G88" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" s="1">
         <v>89</v>
       </c>
       <c r="B89" s="1">
-        <v>765207</v>
+        <v>765314</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="D89" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E89" s="1">
-        <v>1565024</v>
+        <v>1565025</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="G89" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="1">
+    <row r="90" spans="1:7" s="11" customFormat="1">
+      <c r="A90" s="7">
         <v>90</v>
       </c>
-      <c r="B90" s="1">
-        <v>765314</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D90" s="1">
-        <v>3</v>
-      </c>
-      <c r="E90" s="1">
-        <v>1565025</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G90" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="7">
+      <c r="B90" s="7">
+        <v>765202</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D90" s="7">
+        <v>3</v>
+      </c>
+      <c r="E90" s="7">
+        <v>1565026</v>
+      </c>
+      <c r="F90" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G90" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="1">
         <v>91</v>
       </c>
-      <c r="B91" s="7">
-        <v>765202</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D91" s="7">
-        <v>3</v>
-      </c>
-      <c r="E91" s="7">
-        <v>1565026</v>
-      </c>
-      <c r="F91" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G91" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B91" s="1">
+        <v>765310</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D91" s="1">
+        <v>2</v>
+      </c>
+      <c r="E91" s="1">
+        <v>1565027</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G91" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" s="1">
         <v>92</v>
       </c>
       <c r="B92" s="1">
-        <v>765310</v>
+        <v>765215</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D92" s="1">
         <v>2</v>
       </c>
       <c r="E92" s="1">
-        <v>1565027</v>
+        <v>1565028</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G92" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7">
       <c r="A93" s="1">
         <v>93</v>
       </c>
       <c r="B93" s="1">
-        <v>765215</v>
+        <v>765401</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="D93" s="1">
         <v>2</v>
       </c>
       <c r="E93" s="1">
-        <v>1565028</v>
+        <v>1565029</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="G93" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" s="1">
         <v>94</v>
       </c>
       <c r="B94" s="1">
-        <v>765401</v>
+        <v>765404</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D94" s="1">
         <v>2</v>
       </c>
       <c r="E94" s="1">
-        <v>1565029</v>
+        <v>1565030</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="G94" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7">
       <c r="A95" s="1">
         <v>95</v>
       </c>
-      <c r="B95" s="1">
-        <v>765404</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D95" s="1">
-        <v>2</v>
+      <c r="B95" s="5">
+        <v>765405</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D95" s="5">
+        <v>1</v>
       </c>
       <c r="E95" s="1">
-        <v>1565030</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>129</v>
+        <v>1565031</v>
+      </c>
+      <c r="F95" s="8" t="s">
+        <v>144</v>
       </c>
       <c r="G95" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" s="1">
         <v>96</v>
       </c>
@@ -3313,62 +3265,62 @@
         <v>1</v>
       </c>
       <c r="E96" s="1">
-        <v>1565031</v>
+        <v>1565032</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G96" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7">
       <c r="A97" s="1">
         <v>97</v>
       </c>
-      <c r="B97" s="5">
-        <v>765405</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D97" s="5">
+      <c r="B97" s="1">
+        <v>765409</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D97" s="1">
         <v>1</v>
       </c>
       <c r="E97" s="1">
-        <v>1565032</v>
+        <v>1565033</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G97" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7">
       <c r="A98" s="1">
         <v>98</v>
       </c>
-      <c r="B98" s="1">
-        <v>765409</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D98" s="1">
+      <c r="B98" s="5">
+        <v>765410</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D98" s="5">
         <v>1</v>
       </c>
       <c r="E98" s="1">
-        <v>1565033</v>
+        <v>1565034</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G98" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7">
       <c r="A99" s="1">
         <v>99</v>
       </c>
@@ -3382,108 +3334,108 @@
         <v>1</v>
       </c>
       <c r="E99" s="1">
-        <v>1565034</v>
+        <v>1565035</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G99" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7">
       <c r="A100" s="1">
         <v>100</v>
       </c>
-      <c r="B100" s="5">
-        <v>765410</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D100" s="5">
+      <c r="B100" s="1">
+        <v>765406</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D100" s="1">
         <v>1</v>
       </c>
       <c r="E100" s="1">
-        <v>1565035</v>
+        <v>1565036</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G100" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7">
       <c r="A101" s="1">
         <v>101</v>
       </c>
       <c r="B101" s="1">
-        <v>765406</v>
+        <v>765408</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D101" s="1">
         <v>1</v>
       </c>
       <c r="E101" s="1">
-        <v>1565036</v>
+        <v>1565037</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G101" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7">
       <c r="A102" s="1">
         <v>102</v>
       </c>
       <c r="B102" s="1">
-        <v>765408</v>
+        <v>765411</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D102" s="1">
         <v>1</v>
       </c>
       <c r="E102" s="1">
-        <v>1565037</v>
+        <v>1565038</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G102" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7">
       <c r="A103" s="1">
         <v>103</v>
       </c>
-      <c r="B103" s="1">
-        <v>765411</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D103" s="1">
+      <c r="B103" s="5">
+        <v>765415</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D103" s="5">
         <v>1</v>
       </c>
       <c r="E103" s="1">
-        <v>1565038</v>
+        <v>1565039</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G103" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7">
       <c r="A104" s="1">
         <v>104</v>
       </c>
@@ -3497,254 +3449,254 @@
         <v>1</v>
       </c>
       <c r="E104" s="1">
-        <v>1565039</v>
+        <v>1565040</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G104" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7">
       <c r="A105" s="1">
         <v>105</v>
       </c>
-      <c r="B105" s="5">
-        <v>765415</v>
-      </c>
-      <c r="C105" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D105" s="5">
+      <c r="B105" s="1">
+        <v>765414</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D105" s="1">
         <v>1</v>
       </c>
       <c r="E105" s="1">
-        <v>1565040</v>
+        <v>1565041</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G105" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7">
       <c r="A106" s="1">
         <v>106</v>
       </c>
       <c r="B106" s="1">
-        <v>765414</v>
+        <v>765407</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
       <c r="D106" s="1">
         <v>1</v>
       </c>
       <c r="E106" s="1">
-        <v>1565041</v>
+        <v>1565042</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G106" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7">
       <c r="A107" s="1">
         <v>107</v>
       </c>
       <c r="B107" s="1">
-        <v>765407</v>
+        <v>765413</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D107" s="1">
         <v>1</v>
       </c>
       <c r="E107" s="1">
-        <v>1565042</v>
+        <v>1565043</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G107" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7">
       <c r="A108" s="1">
         <v>108</v>
       </c>
       <c r="B108" s="1">
-        <v>765413</v>
+        <v>765412</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D108" s="1">
         <v>1</v>
       </c>
       <c r="E108" s="1">
-        <v>1565043</v>
+        <v>1565044</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G108" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7">
       <c r="A109" s="1">
         <v>109</v>
       </c>
       <c r="B109" s="1">
-        <v>765412</v>
+        <v>765416</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="D109" s="1">
         <v>1</v>
       </c>
       <c r="E109" s="1">
-        <v>1565044</v>
+        <v>1565045</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G109" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7">
       <c r="A110" s="1">
         <v>110</v>
       </c>
       <c r="B110" s="1">
-        <v>765416</v>
+        <v>765501</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="D110" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E110" s="1">
-        <v>1565045</v>
-      </c>
-      <c r="F110" s="8" t="s">
-        <v>158</v>
+        <v>1565046</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="G110" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111" s="1">
         <v>111</v>
       </c>
       <c r="B111" s="1">
-        <v>765501</v>
+        <v>765502</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D111" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E111" s="1">
-        <v>1565046</v>
+        <v>1565047</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G111" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
       <c r="A112" s="1">
         <v>112</v>
       </c>
       <c r="B112" s="1">
-        <v>765502</v>
+        <v>765503</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D112" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E112" s="1">
-        <v>1565047</v>
+        <v>1565048</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G112" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113" s="1">
         <v>113</v>
       </c>
-      <c r="B113" s="1">
-        <v>765503</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D113" s="1">
-        <v>6</v>
+      <c r="B113" s="7">
+        <v>765315</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D113" s="7">
+        <v>3</v>
       </c>
       <c r="E113" s="1">
-        <v>1565048</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>131</v>
+        <v>1565049</v>
+      </c>
+      <c r="F113" s="43" t="s">
+        <v>133</v>
       </c>
       <c r="G113" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" s="12" customFormat="1">
+      <c r="A114" s="5">
         <v>114</v>
       </c>
-      <c r="B114" s="7">
-        <v>765315</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D114" s="7">
-        <v>3</v>
-      </c>
-      <c r="E114" s="1">
-        <v>1565049</v>
-      </c>
-      <c r="F114" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="G114" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B114" s="9">
+        <v>765402</v>
+      </c>
+      <c r="C114" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D114" s="9">
+        <v>2</v>
+      </c>
+      <c r="E114" s="39">
+        <v>1565057</v>
+      </c>
+      <c r="F114" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="G114" s="41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" s="12" customFormat="1">
       <c r="A115" s="5">
         <v>115</v>
       </c>
       <c r="B115" s="9">
-        <v>765402</v>
+        <v>765403</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D115" s="9">
         <v>2</v>
@@ -3759,76 +3711,70 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" s="12" customFormat="1">
       <c r="A116" s="5">
         <v>116</v>
       </c>
       <c r="B116" s="9">
-        <v>765403</v>
+        <v>765304</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D116" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E116" s="39">
-        <v>1565057</v>
+        <v>1565058</v>
       </c>
       <c r="F116" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="G116" s="41">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="G116" s="42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" s="12" customFormat="1">
       <c r="A117" s="5">
         <v>117</v>
       </c>
       <c r="B117" s="9">
-        <v>765304</v>
+        <v>765308</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D117" s="9">
         <v>3</v>
       </c>
-      <c r="E117" s="39">
-        <v>1565058</v>
+      <c r="E117" s="40">
+        <v>1565059</v>
       </c>
       <c r="F117" s="45" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="G117" s="42">
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7">
       <c r="A118" s="5">
         <v>118</v>
       </c>
-      <c r="B118" s="9">
-        <v>765308</v>
-      </c>
-      <c r="C118" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D118" s="9">
-        <v>3</v>
-      </c>
-      <c r="E118" s="40">
-        <v>1565059</v>
-      </c>
-      <c r="F118" s="45" t="s">
-        <v>143</v>
-      </c>
-      <c r="G118" s="42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B118" s="7"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="7"/>
+      <c r="E118" s="1">
+        <v>1565050</v>
+      </c>
+      <c r="F118" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="G118" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
       <c r="A119" s="5">
         <v>119</v>
       </c>
@@ -3836,16 +3782,16 @@
       <c r="C119" s="8"/>
       <c r="D119" s="7"/>
       <c r="E119" s="1">
-        <v>1565050</v>
-      </c>
-      <c r="F119" s="44" t="s">
-        <v>134</v>
+        <v>1565051</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="G119" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7">
       <c r="A120" s="5">
         <v>120</v>
       </c>
@@ -3853,33 +3799,33 @@
       <c r="C120" s="8"/>
       <c r="D120" s="7"/>
       <c r="E120" s="1">
-        <v>1565051</v>
+        <v>1565052</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G120" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7">
       <c r="A121" s="5">
         <v>121</v>
       </c>
-      <c r="B121" s="7"/>
-      <c r="C121" s="8"/>
-      <c r="D121" s="7"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
       <c r="E121" s="1">
-        <v>1565052</v>
+        <v>1565053</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G121" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7">
       <c r="A122" s="5">
         <v>122</v>
       </c>
@@ -3887,16 +3833,16 @@
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
       <c r="E122" s="1">
-        <v>1565053</v>
+        <v>1565054</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G122" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7">
       <c r="A123" s="5">
         <v>123</v>
       </c>
@@ -3904,16 +3850,16 @@
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
       <c r="E123" s="1">
-        <v>1565054</v>
+        <v>1565055</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G123" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7">
       <c r="A124" s="5">
         <v>124</v>
       </c>
@@ -3921,263 +3867,269 @@
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
       <c r="E124" s="1">
-        <v>1565055</v>
+        <v>1565056</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G124" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A125" s="5">
+    <row r="125" spans="1:7">
+      <c r="A125" s="35">
         <v>125</v>
       </c>
-      <c r="B125" s="1"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="1">
-        <v>1565056</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G125" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B125" s="36">
+        <v>1565001</v>
+      </c>
+      <c r="C125" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D125" s="36">
+        <v>2</v>
+      </c>
+      <c r="E125" s="36">
+        <v>1565001</v>
+      </c>
+      <c r="F125" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="G125" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
       <c r="A126" s="35">
         <v>126</v>
       </c>
       <c r="B126" s="36">
-        <v>1565001</v>
+        <v>1565002</v>
       </c>
       <c r="C126" s="37" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D126" s="36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E126" s="36">
-        <v>1565001</v>
+        <v>1565002</v>
       </c>
       <c r="F126" s="37" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G126" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
       <c r="A127" s="35">
         <v>127</v>
       </c>
       <c r="B127" s="36">
-        <v>1565002</v>
+        <v>1565003</v>
       </c>
       <c r="C127" s="37" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="D127" s="36">
         <v>3</v>
       </c>
       <c r="E127" s="36">
-        <v>1565002</v>
+        <v>1565003</v>
       </c>
       <c r="F127" s="37" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="G127" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7">
       <c r="A128" s="35">
         <v>128</v>
       </c>
       <c r="B128" s="36">
-        <v>1565003</v>
+        <v>1565004</v>
       </c>
       <c r="C128" s="37" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="D128" s="36">
         <v>3</v>
       </c>
       <c r="E128" s="36">
-        <v>1565003</v>
+        <v>1565004</v>
       </c>
       <c r="F128" s="37" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="G128" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7">
       <c r="A129" s="35">
         <v>129</v>
       </c>
       <c r="B129" s="36">
-        <v>1565004</v>
+        <v>1565005</v>
       </c>
       <c r="C129" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D129" s="36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E129" s="36">
-        <v>1565004</v>
+        <v>1565005</v>
       </c>
       <c r="F129" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G129" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
       <c r="A130" s="35">
         <v>130</v>
       </c>
       <c r="B130" s="36">
-        <v>1565005</v>
+        <v>1565006</v>
       </c>
       <c r="C130" s="37" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D130" s="36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E130" s="36">
-        <v>1565005</v>
+        <v>1565006</v>
       </c>
       <c r="F130" s="37" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G130" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
       <c r="A131" s="35">
         <v>131</v>
       </c>
       <c r="B131" s="36">
-        <v>1565006</v>
+        <v>1565007</v>
       </c>
       <c r="C131" s="37" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D131" s="36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E131" s="36">
-        <v>1565006</v>
+        <v>1565007</v>
       </c>
       <c r="F131" s="37" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G131" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
       <c r="A132" s="35">
         <v>132</v>
       </c>
       <c r="B132" s="36">
-        <v>1565007</v>
+        <v>1565008</v>
       </c>
       <c r="C132" s="37" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="D132" s="36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E132" s="36">
-        <v>1565007</v>
+        <v>1565008</v>
       </c>
       <c r="F132" s="37" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="G132" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
       <c r="A133" s="35">
         <v>133</v>
       </c>
       <c r="B133" s="36">
-        <v>1565008</v>
+        <v>1565009</v>
       </c>
       <c r="C133" s="37" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="D133" s="36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E133" s="36">
-        <v>1565008</v>
+        <v>1565009</v>
       </c>
       <c r="F133" s="37" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="G133" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
       <c r="A134" s="35">
         <v>134</v>
       </c>
       <c r="B134" s="36">
-        <v>1565009</v>
+        <v>1565010</v>
       </c>
       <c r="C134" s="37" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D134" s="36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E134" s="36">
-        <v>1565009</v>
+        <v>1565010</v>
       </c>
       <c r="F134" s="37" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G134" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
       <c r="A135" s="35">
         <v>135</v>
       </c>
-      <c r="B135" s="36">
-        <v>1565010</v>
-      </c>
-      <c r="C135" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="D135" s="36">
-        <v>3</v>
-      </c>
-      <c r="E135" s="36">
-        <v>1565010</v>
-      </c>
-      <c r="F135" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="G135" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B135" s="35">
+        <v>1565011</v>
+      </c>
+      <c r="C135" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="D135" s="35">
+        <v>3</v>
+      </c>
+      <c r="E135" s="35">
+        <v>1565011</v>
+      </c>
+      <c r="F135" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="G135" s="35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
       <c r="A136" s="35">
         <v>136</v>
       </c>
@@ -4200,30 +4152,30 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7">
       <c r="A137" s="35">
         <v>137</v>
       </c>
       <c r="B137" s="35">
-        <v>1565011</v>
+        <v>1565012</v>
       </c>
       <c r="C137" s="38" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D137" s="35">
         <v>3</v>
       </c>
       <c r="E137" s="35">
-        <v>1565011</v>
+        <v>1565012</v>
       </c>
       <c r="F137" s="38" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G137" s="35">
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7">
       <c r="A138" s="35">
         <v>138</v>
       </c>
@@ -4246,76 +4198,76 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7">
       <c r="A139" s="35">
         <v>139</v>
       </c>
-      <c r="B139" s="35">
-        <v>1565012</v>
-      </c>
-      <c r="C139" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="D139" s="35">
-        <v>3</v>
-      </c>
-      <c r="E139" s="35">
-        <v>1565012</v>
-      </c>
-      <c r="F139" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="G139" s="35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B139" s="36">
+        <v>1565013</v>
+      </c>
+      <c r="C139" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="D139" s="36">
+        <v>2</v>
+      </c>
+      <c r="E139" s="36">
+        <v>1565013</v>
+      </c>
+      <c r="F139" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="G139" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
       <c r="A140" s="35">
         <v>140</v>
       </c>
       <c r="B140" s="36">
-        <v>1565013</v>
+        <v>1565014</v>
       </c>
       <c r="C140" s="37" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="D140" s="36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E140" s="36">
-        <v>1565013</v>
+        <v>1565014</v>
       </c>
       <c r="F140" s="37" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G140" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
       <c r="A141" s="35">
         <v>141</v>
       </c>
-      <c r="B141" s="36">
-        <v>1565014</v>
-      </c>
-      <c r="C141" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="D141" s="36">
-        <v>3</v>
-      </c>
-      <c r="E141" s="36">
-        <v>1565014</v>
-      </c>
-      <c r="F141" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="G141" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B141" s="35">
+        <v>1565015</v>
+      </c>
+      <c r="C141" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="D141" s="35">
+        <v>3</v>
+      </c>
+      <c r="E141" s="35">
+        <v>1565015</v>
+      </c>
+      <c r="F141" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="G141" s="35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
       <c r="A142" s="35">
         <v>142</v>
       </c>
@@ -4338,812 +4290,812 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7">
       <c r="A143" s="35">
         <v>143</v>
       </c>
-      <c r="B143" s="35">
-        <v>1565015</v>
-      </c>
-      <c r="C143" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="D143" s="35">
-        <v>3</v>
-      </c>
-      <c r="E143" s="35">
-        <v>1565015</v>
-      </c>
-      <c r="F143" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="G143" s="35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B143" s="36">
+        <v>1565016</v>
+      </c>
+      <c r="C143" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="D143" s="36">
+        <v>2</v>
+      </c>
+      <c r="E143" s="36">
+        <v>1565016</v>
+      </c>
+      <c r="F143" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="G143" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
       <c r="A144" s="35">
         <v>144</v>
       </c>
       <c r="B144" s="36">
-        <v>1565016</v>
+        <v>1565017</v>
       </c>
       <c r="C144" s="37" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="D144" s="36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E144" s="36">
-        <v>1565016</v>
+        <v>1565017</v>
       </c>
       <c r="F144" s="37" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="G144" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
       <c r="A145" s="35">
         <v>145</v>
       </c>
       <c r="B145" s="36">
-        <v>1565017</v>
+        <v>1565018</v>
       </c>
       <c r="C145" s="37" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D145" s="36">
         <v>3</v>
       </c>
       <c r="E145" s="36">
-        <v>1565017</v>
+        <v>1565018</v>
       </c>
       <c r="F145" s="37" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="G145" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7">
       <c r="A146" s="35">
         <v>146</v>
       </c>
       <c r="B146" s="36">
-        <v>1565018</v>
+        <v>1565019</v>
       </c>
       <c r="C146" s="37" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D146" s="36">
         <v>3</v>
       </c>
       <c r="E146" s="36">
-        <v>1565018</v>
+        <v>1565019</v>
       </c>
       <c r="F146" s="37" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G146" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7">
       <c r="A147" s="35">
         <v>147</v>
       </c>
       <c r="B147" s="36">
-        <v>1565019</v>
+        <v>1565020</v>
       </c>
       <c r="C147" s="37" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D147" s="36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E147" s="36">
-        <v>1565019</v>
+        <v>1565020</v>
       </c>
       <c r="F147" s="37" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="G147" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
       <c r="A148" s="35">
         <v>148</v>
       </c>
       <c r="B148" s="36">
-        <v>1565020</v>
+        <v>1565021</v>
       </c>
       <c r="C148" s="37" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="D148" s="36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E148" s="36">
-        <v>1565020</v>
+        <v>1565021</v>
       </c>
       <c r="F148" s="37" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="G148" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
       <c r="A149" s="35">
         <v>149</v>
       </c>
       <c r="B149" s="36">
-        <v>1565021</v>
+        <v>1565022</v>
       </c>
       <c r="C149" s="37" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="D149" s="36">
         <v>3</v>
       </c>
       <c r="E149" s="36">
-        <v>1565021</v>
+        <v>1565022</v>
       </c>
       <c r="F149" s="37" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="G149" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7">
       <c r="A150" s="35">
         <v>150</v>
       </c>
       <c r="B150" s="36">
-        <v>1565022</v>
+        <v>1565023</v>
       </c>
       <c r="C150" s="37" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="D150" s="36">
         <v>3</v>
       </c>
       <c r="E150" s="36">
-        <v>1565022</v>
+        <v>1565023</v>
       </c>
       <c r="F150" s="37" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="G150" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7">
       <c r="A151" s="35">
         <v>151</v>
       </c>
       <c r="B151" s="36">
-        <v>1565023</v>
+        <v>1565024</v>
       </c>
       <c r="C151" s="37" t="s">
-        <v>141</v>
+        <v>82</v>
       </c>
       <c r="D151" s="36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E151" s="36">
-        <v>1565023</v>
+        <v>1565024</v>
       </c>
       <c r="F151" s="37" t="s">
-        <v>141</v>
+        <v>82</v>
       </c>
       <c r="G151" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
       <c r="A152" s="35">
         <v>152</v>
       </c>
       <c r="B152" s="36">
-        <v>1565024</v>
+        <v>1565025</v>
       </c>
       <c r="C152" s="37" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="D152" s="36">
         <v>2</v>
       </c>
       <c r="E152" s="36">
-        <v>1565024</v>
+        <v>1565025</v>
       </c>
       <c r="F152" s="37" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="G152" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7">
       <c r="A153" s="35">
         <v>153</v>
       </c>
       <c r="B153" s="36">
-        <v>1565025</v>
+        <v>1565026</v>
       </c>
       <c r="C153" s="37" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D153" s="36">
         <v>2</v>
       </c>
       <c r="E153" s="36">
-        <v>1565025</v>
+        <v>1565026</v>
       </c>
       <c r="F153" s="37" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G153" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7">
       <c r="A154" s="35">
         <v>154</v>
       </c>
       <c r="B154" s="36">
-        <v>1565026</v>
+        <v>1565027</v>
       </c>
       <c r="C154" s="37" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D154" s="36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E154" s="36">
-        <v>1565026</v>
+        <v>1565027</v>
       </c>
       <c r="F154" s="37" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G154" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
       <c r="A155" s="35">
         <v>155</v>
       </c>
       <c r="B155" s="36">
-        <v>1565027</v>
+        <v>1565028</v>
       </c>
       <c r="C155" s="37" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D155" s="36">
         <v>3</v>
       </c>
       <c r="E155" s="36">
-        <v>1565027</v>
+        <v>1565028</v>
       </c>
       <c r="F155" s="37" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G155" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7">
       <c r="A156" s="35">
         <v>156</v>
       </c>
       <c r="B156" s="36">
-        <v>1565028</v>
+        <v>1565029</v>
       </c>
       <c r="C156" s="37" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D156" s="36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E156" s="36">
-        <v>1565028</v>
+        <v>1565029</v>
       </c>
       <c r="F156" s="37" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="G156" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
       <c r="A157" s="35">
         <v>157</v>
       </c>
       <c r="B157" s="36">
-        <v>1565029</v>
+        <v>1565030</v>
       </c>
       <c r="C157" s="37" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="D157" s="36">
         <v>2</v>
       </c>
       <c r="E157" s="36">
-        <v>1565029</v>
+        <v>1565030</v>
       </c>
       <c r="F157" s="37" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="G157" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7">
       <c r="A158" s="35">
         <v>158</v>
       </c>
       <c r="B158" s="36">
-        <v>1565030</v>
+        <v>1565031</v>
       </c>
       <c r="C158" s="37" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="D158" s="36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E158" s="36">
-        <v>1565030</v>
+        <v>1565031</v>
       </c>
       <c r="F158" s="37" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="G158" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
       <c r="A159" s="35">
         <v>159</v>
       </c>
       <c r="B159" s="36">
-        <v>1565031</v>
+        <v>1565032</v>
       </c>
       <c r="C159" s="37" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D159" s="36">
         <v>1</v>
       </c>
       <c r="E159" s="36">
-        <v>1565031</v>
+        <v>1565032</v>
       </c>
       <c r="F159" s="37" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G159" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7">
       <c r="A160" s="35">
         <v>160</v>
       </c>
       <c r="B160" s="36">
-        <v>1565032</v>
+        <v>1565033</v>
       </c>
       <c r="C160" s="37" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D160" s="36">
         <v>1</v>
       </c>
       <c r="E160" s="36">
-        <v>1565032</v>
+        <v>1565033</v>
       </c>
       <c r="F160" s="37" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G160" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7">
       <c r="A161" s="35">
         <v>161</v>
       </c>
       <c r="B161" s="36">
-        <v>1565033</v>
+        <v>1565034</v>
       </c>
       <c r="C161" s="37" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D161" s="36">
         <v>1</v>
       </c>
       <c r="E161" s="36">
-        <v>1565033</v>
+        <v>1565034</v>
       </c>
       <c r="F161" s="37" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G161" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7">
       <c r="A162" s="35">
         <v>162</v>
       </c>
       <c r="B162" s="36">
-        <v>1565034</v>
+        <v>1565035</v>
       </c>
       <c r="C162" s="37" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D162" s="36">
         <v>1</v>
       </c>
       <c r="E162" s="36">
-        <v>1565034</v>
+        <v>1565035</v>
       </c>
       <c r="F162" s="37" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G162" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7">
       <c r="A163" s="35">
         <v>163</v>
       </c>
       <c r="B163" s="36">
-        <v>1565035</v>
+        <v>1565036</v>
       </c>
       <c r="C163" s="37" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D163" s="36">
         <v>1</v>
       </c>
       <c r="E163" s="36">
-        <v>1565035</v>
+        <v>1565036</v>
       </c>
       <c r="F163" s="37" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G163" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7">
       <c r="A164" s="35">
         <v>164</v>
       </c>
       <c r="B164" s="36">
-        <v>1565036</v>
+        <v>1565037</v>
       </c>
       <c r="C164" s="37" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D164" s="36">
         <v>1</v>
       </c>
       <c r="E164" s="36">
-        <v>1565036</v>
+        <v>1565037</v>
       </c>
       <c r="F164" s="37" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G164" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7">
       <c r="A165" s="35">
         <v>165</v>
       </c>
       <c r="B165" s="36">
-        <v>1565037</v>
+        <v>1565038</v>
       </c>
       <c r="C165" s="37" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D165" s="36">
         <v>1</v>
       </c>
       <c r="E165" s="36">
-        <v>1565037</v>
+        <v>1565038</v>
       </c>
       <c r="F165" s="37" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G165" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7">
       <c r="A166" s="35">
         <v>166</v>
       </c>
       <c r="B166" s="36">
-        <v>1565038</v>
+        <v>1565039</v>
       </c>
       <c r="C166" s="37" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D166" s="36">
         <v>1</v>
       </c>
       <c r="E166" s="36">
-        <v>1565038</v>
+        <v>1565039</v>
       </c>
       <c r="F166" s="37" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G166" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7">
       <c r="A167" s="35">
         <v>167</v>
       </c>
       <c r="B167" s="36">
-        <v>1565039</v>
+        <v>1565040</v>
       </c>
       <c r="C167" s="37" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D167" s="36">
         <v>1</v>
       </c>
       <c r="E167" s="36">
-        <v>1565039</v>
+        <v>1565040</v>
       </c>
       <c r="F167" s="37" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G167" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7">
       <c r="A168" s="35">
         <v>168</v>
       </c>
       <c r="B168" s="36">
-        <v>1565040</v>
+        <v>1565041</v>
       </c>
       <c r="C168" s="37" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D168" s="36">
         <v>1</v>
       </c>
       <c r="E168" s="36">
-        <v>1565040</v>
+        <v>1565041</v>
       </c>
       <c r="F168" s="37" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G168" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7">
       <c r="A169" s="35">
         <v>169</v>
       </c>
       <c r="B169" s="36">
-        <v>1565041</v>
+        <v>1565042</v>
       </c>
       <c r="C169" s="37" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D169" s="36">
         <v>1</v>
       </c>
       <c r="E169" s="36">
-        <v>1565041</v>
+        <v>1565042</v>
       </c>
       <c r="F169" s="37" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G169" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7">
       <c r="A170" s="35">
         <v>170</v>
       </c>
       <c r="B170" s="36">
-        <v>1565042</v>
+        <v>1565043</v>
       </c>
       <c r="C170" s="37" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D170" s="36">
         <v>1</v>
       </c>
       <c r="E170" s="36">
-        <v>1565042</v>
+        <v>1565043</v>
       </c>
       <c r="F170" s="37" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G170" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7">
       <c r="A171" s="35">
         <v>171</v>
       </c>
       <c r="B171" s="36">
-        <v>1565043</v>
+        <v>1565044</v>
       </c>
       <c r="C171" s="37" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D171" s="36">
         <v>1</v>
       </c>
       <c r="E171" s="36">
-        <v>1565043</v>
+        <v>1565044</v>
       </c>
       <c r="F171" s="37" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G171" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7">
       <c r="A172" s="35">
         <v>172</v>
       </c>
       <c r="B172" s="36">
-        <v>1565044</v>
+        <v>1565045</v>
       </c>
       <c r="C172" s="37" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D172" s="36">
         <v>1</v>
       </c>
       <c r="E172" s="36">
-        <v>1565044</v>
+        <v>1565045</v>
       </c>
       <c r="F172" s="37" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G172" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7">
       <c r="A173" s="35">
         <v>173</v>
       </c>
       <c r="B173" s="36">
-        <v>1565045</v>
+        <v>1565046</v>
       </c>
       <c r="C173" s="37" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="D173" s="36">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E173" s="36">
-        <v>1565045</v>
+        <v>1565046</v>
       </c>
       <c r="F173" s="37" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="G173" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7">
       <c r="A174" s="35">
         <v>174</v>
       </c>
       <c r="B174" s="36">
-        <v>1565046</v>
+        <v>1565047</v>
       </c>
       <c r="C174" s="37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D174" s="36">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E174" s="36">
-        <v>1565046</v>
+        <v>1565047</v>
       </c>
       <c r="F174" s="37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G174" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7">
       <c r="A175" s="35">
         <v>175</v>
       </c>
       <c r="B175" s="36">
-        <v>1565047</v>
+        <v>1565048</v>
       </c>
       <c r="C175" s="37" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D175" s="36">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E175" s="36">
-        <v>1565047</v>
+        <v>1565048</v>
       </c>
       <c r="F175" s="37" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G175" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7">
       <c r="A176" s="35">
         <v>176</v>
       </c>
       <c r="B176" s="36">
-        <v>1565048</v>
-      </c>
-      <c r="C176" s="37" t="s">
-        <v>131</v>
+        <v>1565049</v>
+      </c>
+      <c r="C176" s="48" t="s">
+        <v>133</v>
       </c>
       <c r="D176" s="36">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E176" s="36">
-        <v>1565048</v>
-      </c>
-      <c r="F176" s="37" t="s">
-        <v>131</v>
+        <v>1565049</v>
+      </c>
+      <c r="F176" s="48" t="s">
+        <v>133</v>
       </c>
       <c r="G176" s="36">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7">
       <c r="A177" s="35">
         <v>177</v>
       </c>
-      <c r="B177" s="36">
-        <v>1565049</v>
-      </c>
-      <c r="C177" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="D177" s="36">
-        <v>3</v>
-      </c>
-      <c r="E177" s="36">
-        <v>1565049</v>
-      </c>
-      <c r="F177" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="G177" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B177" s="46">
+        <v>1565057</v>
+      </c>
+      <c r="C177" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="D177" s="47">
+        <v>3</v>
+      </c>
+      <c r="E177" s="46">
+        <v>1565057</v>
+      </c>
+      <c r="F177" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="G177" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7">
       <c r="A178" s="35">
         <v>178</v>
       </c>
@@ -5166,239 +5118,216 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7">
       <c r="A179" s="35">
         <v>179</v>
       </c>
       <c r="B179" s="46">
-        <v>1565057</v>
+        <v>1565058</v>
       </c>
       <c r="C179" s="50" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="D179" s="47">
         <v>3</v>
       </c>
       <c r="E179" s="46">
-        <v>1565057</v>
+        <v>1565058</v>
       </c>
       <c r="F179" s="50" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="G179" s="47">
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7">
       <c r="A180" s="35">
         <v>180</v>
       </c>
       <c r="B180" s="46">
-        <v>1565058</v>
+        <v>1565059</v>
       </c>
       <c r="C180" s="50" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="D180" s="47">
         <v>3</v>
       </c>
       <c r="E180" s="46">
-        <v>1565058</v>
+        <v>1565059</v>
       </c>
       <c r="F180" s="50" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="G180" s="47">
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7">
       <c r="A181" s="35">
         <v>181</v>
       </c>
-      <c r="B181" s="46">
-        <v>1565059</v>
-      </c>
-      <c r="C181" s="50" t="s">
-        <v>143</v>
-      </c>
-      <c r="D181" s="47">
-        <v>3</v>
-      </c>
-      <c r="E181" s="46">
-        <v>1565059</v>
-      </c>
-      <c r="F181" s="50" t="s">
-        <v>143</v>
-      </c>
-      <c r="G181" s="47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B181" s="36">
+        <v>1565050</v>
+      </c>
+      <c r="C181" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="D181" s="36">
+        <v>3</v>
+      </c>
+      <c r="E181" s="36">
+        <v>1565050</v>
+      </c>
+      <c r="F181" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="G181" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7">
       <c r="A182" s="35">
         <v>182</v>
       </c>
       <c r="B182" s="36">
-        <v>1565050</v>
-      </c>
-      <c r="C182" s="49" t="s">
-        <v>134</v>
+        <v>1565051</v>
+      </c>
+      <c r="C182" s="37" t="s">
+        <v>135</v>
       </c>
       <c r="D182" s="36">
         <v>3</v>
       </c>
       <c r="E182" s="36">
-        <v>1565050</v>
-      </c>
-      <c r="F182" s="49" t="s">
-        <v>134</v>
+        <v>1565051</v>
+      </c>
+      <c r="F182" s="37" t="s">
+        <v>135</v>
       </c>
       <c r="G182" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7">
       <c r="A183" s="35">
         <v>183</v>
       </c>
       <c r="B183" s="36">
-        <v>1565051</v>
+        <v>1565052</v>
       </c>
       <c r="C183" s="37" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D183" s="36">
         <v>3</v>
       </c>
       <c r="E183" s="36">
-        <v>1565051</v>
+        <v>1565052</v>
       </c>
       <c r="F183" s="37" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G183" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7">
       <c r="A184" s="35">
         <v>184</v>
       </c>
       <c r="B184" s="36">
-        <v>1565052</v>
+        <v>1565053</v>
       </c>
       <c r="C184" s="37" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D184" s="36">
         <v>3</v>
       </c>
       <c r="E184" s="36">
-        <v>1565052</v>
+        <v>1565053</v>
       </c>
       <c r="F184" s="37" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G184" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7">
       <c r="A185" s="35">
         <v>185</v>
       </c>
       <c r="B185" s="36">
-        <v>1565053</v>
+        <v>1565054</v>
       </c>
       <c r="C185" s="37" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D185" s="36">
         <v>3</v>
       </c>
       <c r="E185" s="36">
-        <v>1565053</v>
+        <v>1565054</v>
       </c>
       <c r="F185" s="37" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G185" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7">
       <c r="A186" s="35">
         <v>186</v>
       </c>
       <c r="B186" s="36">
-        <v>1565054</v>
+        <v>1565055</v>
       </c>
       <c r="C186" s="37" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D186" s="36">
         <v>3</v>
       </c>
       <c r="E186" s="36">
-        <v>1565054</v>
+        <v>1565055</v>
       </c>
       <c r="F186" s="37" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G186" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7">
       <c r="A187" s="35">
         <v>187</v>
       </c>
       <c r="B187" s="36">
-        <v>1565055</v>
+        <v>1565056</v>
       </c>
       <c r="C187" s="37" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D187" s="36">
         <v>3</v>
       </c>
       <c r="E187" s="36">
-        <v>1565055</v>
+        <v>1565056</v>
       </c>
       <c r="F187" s="37" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G187" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A188" s="35">
-        <v>188</v>
-      </c>
-      <c r="B188" s="36">
-        <v>1565056</v>
-      </c>
-      <c r="C188" s="37" t="s">
-        <v>140</v>
-      </c>
-      <c r="D188" s="36">
-        <v>3</v>
-      </c>
-      <c r="E188" s="36">
-        <v>1565056</v>
-      </c>
-      <c r="F188" s="37" t="s">
-        <v>140</v>
-      </c>
-      <c r="G188" s="36">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="95" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="95" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="43" max="16383" man="1"/>
   </rowBreaks>

</xml_diff>